<commit_message>
Cleaning and Flushing Mode (Automation)
</commit_message>
<xml_diff>
--- a/recipeCreationVacuumMode.xlsx
+++ b/recipeCreationVacuumMode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lattice\Desktop\ss\RecipeCreation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87ECCBF0-A675-4710-A410-BA7E1C8E1E2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8105BB3-0D62-40F4-8D37-D8AA7E02C384}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="753" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="196">
   <si>
     <t>UC_ID</t>
   </si>
@@ -595,15 +595,6 @@
   </si>
   <si>
     <t>KrosFlo FS 500</t>
-  </si>
-  <si>
-    <t>toastMessage</t>
-  </si>
-  <si>
-    <t>captureMessage</t>
-  </si>
-  <si>
-    <t>Recipe created</t>
   </si>
   <si>
     <t>KR2i_Vacuum</t>
@@ -1151,10 +1142,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06968273-B5FF-4DDF-9616-03EB7EEDE40B}">
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1212,8 +1203,8 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
+      <c r="G2" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="H2" s="10"/>
     </row>
@@ -1236,8 +1227,8 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
-        <v>13</v>
+      <c r="G3" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="H3" s="7"/>
     </row>
@@ -1260,8 +1251,8 @@
       <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
-        <v>13</v>
+      <c r="G4" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="H4" s="7"/>
     </row>
@@ -1284,8 +1275,8 @@
       <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" t="s">
-        <v>13</v>
+      <c r="G5" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="H5" s="7"/>
     </row>
@@ -1308,8 +1299,8 @@
       <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" t="s">
-        <v>13</v>
+      <c r="G6" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -1418,7 +1409,7 @@
         <v>17</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>35</v>
@@ -1442,7 +1433,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>36</v>
@@ -1460,7 +1451,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -1469,7 +1460,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>13</v>
@@ -2255,7 +2246,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C47" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D47" t="s">
         <v>159</v>
@@ -2264,7 +2255,7 @@
         <v>12</v>
       </c>
       <c r="F47" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G47" t="s">
         <v>13</v>
@@ -3049,30 +3040,7 @@
         <v>110</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A82">
-        <v>1.4</v>
-      </c>
-      <c r="B82">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C82" t="s">
-        <v>111</v>
-      </c>
-      <c r="D82" t="s">
-        <v>188</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="F82" t="s">
-        <v>187</v>
-      </c>
-      <c r="G82" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3089,8 +3057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72D330A-C15D-4736-9D57-120BD7CA4F73}">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3148,7 +3116,7 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H2" s="10"/>
@@ -3172,7 +3140,7 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="7"/>
@@ -3196,7 +3164,7 @@
       <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="7"/>
@@ -3220,7 +3188,7 @@
       <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H5" s="7"/>
@@ -3244,7 +3212,7 @@
       <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H6" s="7"/>
@@ -3354,7 +3322,7 @@
         <v>17</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>35</v>
@@ -3378,7 +3346,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>36</v>
@@ -3396,7 +3364,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -3405,7 +3373,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>13</v>
@@ -4191,7 +4159,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C47" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D47" t="s">
         <v>159</v>
@@ -4200,7 +4168,7 @@
         <v>12</v>
       </c>
       <c r="F47" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G47" t="s">
         <v>13</v>
@@ -4985,7 +4953,7 @@
         <v>110</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -5000,8 +4968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E855714-9B39-4CC2-A9F7-DB85BBFA9633}">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5265,7 +5233,7 @@
         <v>17</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>35</v>
@@ -5289,7 +5257,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>36</v>
@@ -5307,7 +5275,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -5316,7 +5284,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>13</v>
@@ -6102,7 +6070,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C47" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D47" t="s">
         <v>159</v>
@@ -6111,7 +6079,7 @@
         <v>12</v>
       </c>
       <c r="F47" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G47" t="s">
         <v>13</v>
@@ -6896,7 +6864,7 @@
         <v>110</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -6911,8 +6879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353F7C62-A3A7-4A3F-974E-A86CAAC2D3EE}">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7176,7 +7144,7 @@
         <v>17</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>35</v>
@@ -7200,7 +7168,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>36</v>
@@ -7218,7 +7186,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -7227,7 +7195,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>13</v>
@@ -8013,7 +7981,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C47" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D47" t="s">
         <v>159</v>
@@ -8022,7 +7990,7 @@
         <v>12</v>
       </c>
       <c r="F47" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G47" t="s">
         <v>13</v>
@@ -8807,7 +8775,7 @@
         <v>110</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>